<commit_message>
Aniado ficheros evaluacion 1 y evaluacion 2 con analisis denso automatico
</commit_message>
<xml_diff>
--- a/Evaluacion 2/results/DECA/est_error_DECA.xlsx
+++ b/Evaluacion 2/results/DECA/est_error_DECA.xlsx
@@ -763,25 +763,25 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13">
-        <v>6.066856002566657</v>
+        <v>5.976345840007698</v>
       </c>
       <c r="D13">
-        <v>2.890014841222408</v>
+        <v>2.850519313807858</v>
       </c>
       <c r="E13">
         <v>1.842283931653768</v>
       </c>
       <c r="F13">
-        <v>4.110424673988464</v>
+        <v>3.928635258818658</v>
       </c>
       <c r="G13">
         <v>5.68408256110693</v>
       </c>
       <c r="H13">
-        <v>7.726898306680637</v>
+        <v>7.616757027140137</v>
       </c>
       <c r="I13">
         <v>13.29890047346921</v>

</xml_diff>